<commit_message>
a lot of improvements
</commit_message>
<xml_diff>
--- a/admin/Student_details/2021-06-23Student_details.xlsx
+++ b/admin/Student_details/2021-06-23Student_details.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="35">
   <si>
     <t>Gr no.</t>
   </si>
@@ -69,14 +69,14 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">123234345657879765</t>
+      <t xml:space="preserve">768798765456554376</t>
     </r>
   </si>
   <si>
-    <t>chavda priya p.</t>
-  </si>
-  <si>
-    <t>-</t>
+    <t>gor tisha a.</t>
+  </si>
+  <si>
+    <t>Arts</t>
   </si>
   <si>
     <t>hindu</t>
@@ -85,21 +85,18 @@
     <t>ST</t>
   </si>
   <si>
-    <t>2001-10-23</t>
-  </si>
-  <si>
-    <t>2018-07-14</t>
+    <t>2005-05-17</t>
+  </si>
+  <si>
+    <t>2018-07-17</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">874567465746</t>
+      <t xml:space="preserve">234576238798</t>
     </r>
   </si>
   <si>
-    <t>halaynagar,madhapar</t>
-  </si>
-  <si>
-    <t>lohana hostel</t>
+    <t>sayognagar,bhuj</t>
   </si>
   <si>
     <t>No</t>
@@ -109,103 +106,28 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">345456567678987654</t>
+      <t xml:space="preserve">567678909876543234</t>
     </r>
   </si>
   <si>
-    <t>nai rutva d.</t>
-  </si>
-  <si>
-    <t>OBC</t>
-  </si>
-  <si>
-    <t>2010-07-07</t>
-  </si>
-  <si>
-    <t>2018-07-19</t>
+    <t>sukla hetal u.</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>2008-02-20</t>
+  </si>
+  <si>
+    <t>2018-07-31</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">098987456787</t>
+      <t xml:space="preserve">902348599598</t>
     </r>
   </si>
   <si>
-    <t>saktidham,mirjapar</t>
-  </si>
-  <si>
-    <t>YES</t>
-  </si>
-  <si>
-    <t>Deaf</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">987654345678909876</t>
-    </r>
-  </si>
-  <si>
-    <t>gohil kinjal dhavalbhai</t>
-  </si>
-  <si>
-    <t>General</t>
-  </si>
-  <si>
-    <t>2006-04-05</t>
-  </si>
-  <si>
-    <t>2018-07-21</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">984578342378</t>
-    </r>
-  </si>
-  <si>
-    <t>bharvad vas, bhuj</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">656765434567865432</t>
-    </r>
-  </si>
-  <si>
-    <t>morabiya geeta n.</t>
-  </si>
-  <si>
-    <t>2007-01-02</t>
-  </si>
-  <si>
-    <t>2018-07-26</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">123856986567</t>
-    </r>
-  </si>
-  <si>
-    <t>prbhunagar,bhuj</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">456787656885432467</t>
-    </r>
-  </si>
-  <si>
-    <t>thackerr mina i.</t>
-  </si>
-  <si>
-    <t>2002-04-30</t>
-  </si>
-  <si>
-    <t>2018-07-30</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">648373728372</t>
-    </r>
-  </si>
-  <si>
-    <t>kodkiroad,bhuj</t>
+    <t>kalitash,bhuj</t>
   </si>
 </sst>
 </file>
@@ -544,7 +466,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:Q6"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -554,7 +476,7 @@
   <cols>
     <col min="1" max="1" width="8.140869" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="22.280273" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="28.135986" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="17.567139" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="6.998291" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="8.140869" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="6.998291" bestFit="true" customWidth="true" style="0"/>
@@ -563,7 +485,7 @@
     <col min="9" max="9" width="17.567139" bestFit="true" customWidth="true" style="0"/>
     <col min="10" max="10" width="13.996582" bestFit="true" customWidth="true" style="0"/>
     <col min="11" max="11" width="15.281982" bestFit="true" customWidth="true" style="0"/>
-    <col min="12" max="12" width="23.422852" bestFit="true" customWidth="true" style="0"/>
+    <col min="12" max="12" width="18.709717" bestFit="true" customWidth="true" style="0"/>
     <col min="13" max="13" width="17.567139" bestFit="true" customWidth="true" style="0"/>
     <col min="14" max="14" width="13.996582" bestFit="true" customWidth="true" style="0"/>
     <col min="15" max="15" width="10.568848" bestFit="true" customWidth="true" style="0"/>
@@ -626,12 +548,12 @@
     </row>
     <row r="2" spans="1:17">
       <c r="A2">
-        <v>97172</v>
+        <v>72637</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">123234345657879765</t>
+            <t xml:space="preserve">768798765456554376</t>
           </r>
         </is>
       </c>
@@ -639,7 +561,7 @@
         <v>18</v>
       </c>
       <c r="D2">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
         <v>19</v>
@@ -657,46 +579,44 @@
         <v>23</v>
       </c>
       <c r="J2">
-        <v>1232312312</v>
+        <v>9876543210</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">874567465746</t>
+            <t xml:space="preserve">234576238798</t>
           </r>
         </is>
       </c>
       <c r="L2" t="s">
         <v>25</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2"/>
+      <c r="N2" t="s">
         <v>26</v>
-      </c>
-      <c r="N2" t="s">
-        <v>27</v>
       </c>
       <c r="O2"/>
       <c r="P2"/>
       <c r="Q2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:17">
       <c r="A3">
-        <v>12382</v>
+        <v>65463</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">345456567678987654</t>
+            <t xml:space="preserve">567678909876543234</t>
           </r>
         </is>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D3">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
         <v>19</v>
@@ -705,206 +625,35 @@
         <v>20</v>
       </c>
       <c r="G3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" t="s">
         <v>31</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>32</v>
       </c>
-      <c r="I3" t="s">
-        <v>33</v>
-      </c>
       <c r="J3">
-        <v>7878786645</v>
+        <v>6858443344</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">098987456787</t>
+            <t xml:space="preserve">902348599598</t>
           </r>
         </is>
       </c>
       <c r="L3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M3"/>
       <c r="N3" t="s">
-        <v>36</v>
-      </c>
-      <c r="O3" t="s">
-        <v>37</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="O3"/>
       <c r="P3"/>
       <c r="Q3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17">
-      <c r="A4">
-        <v>97263</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">987654345678909876</t>
-          </r>
-        </is>
-      </c>
-      <c r="C4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4">
-        <v>9</v>
-      </c>
-      <c r="E4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" t="s">
-        <v>40</v>
-      </c>
-      <c r="H4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I4" t="s">
-        <v>42</v>
-      </c>
-      <c r="J4">
-        <v>1232131233</v>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">984578342378</t>
-          </r>
-        </is>
-      </c>
-      <c r="L4" t="s">
-        <v>44</v>
-      </c>
-      <c r="M4" t="s">
-        <v>26</v>
-      </c>
-      <c r="N4" t="s">
         <v>27</v>
-      </c>
-      <c r="O4"/>
-      <c r="P4"/>
-      <c r="Q4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
-      <c r="A5">
-        <v>72828</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">656765434567865432</t>
-          </r>
-        </is>
-      </c>
-      <c r="C5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5">
-        <v>9</v>
-      </c>
-      <c r="E5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" t="s">
-        <v>47</v>
-      </c>
-      <c r="I5" t="s">
-        <v>48</v>
-      </c>
-      <c r="J5">
-        <v>4534454443</v>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">123856986567</t>
-          </r>
-        </is>
-      </c>
-      <c r="L5" t="s">
-        <v>50</v>
-      </c>
-      <c r="M5"/>
-      <c r="N5" t="s">
-        <v>27</v>
-      </c>
-      <c r="O5"/>
-      <c r="P5"/>
-      <c r="Q5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17">
-      <c r="A6">
-        <v>73784</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">456787656885432467</t>
-          </r>
-        </is>
-      </c>
-      <c r="C6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D6">
-        <v>9</v>
-      </c>
-      <c r="E6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H6" t="s">
-        <v>53</v>
-      </c>
-      <c r="I6" t="s">
-        <v>54</v>
-      </c>
-      <c r="J6">
-        <v>3423423432</v>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">648373728372</t>
-          </r>
-        </is>
-      </c>
-      <c r="L6" t="s">
-        <v>56</v>
-      </c>
-      <c r="M6"/>
-      <c r="N6" t="s">
-        <v>36</v>
-      </c>
-      <c r="O6" t="s">
-        <v>37</v>
-      </c>
-      <c r="P6"/>
-      <c r="Q6" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>